<commit_message>
Worked on results graphs
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="627" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="628" uniqueCount="12">
   <si>
     <t>MazeNumber</t>
   </si>
@@ -58,6 +58,9 @@
   </si>
   <si>
     <t>Manhatten Distance</t>
+  </si>
+  <si>
+    <t>Min</t>
   </si>
 </sst>
 </file>
@@ -106,14 +109,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -14893,7 +14896,7 @@
   <dimension ref="A1:X152"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="X10" sqref="X10"/>
+      <selection activeCell="V6" sqref="V6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -14921,30 +14924,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="4"/>
-      <c r="G1" s="2" t="s">
+      <c r="C1" s="3"/>
+      <c r="G1" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="H1" s="2"/>
-      <c r="L1" s="2" t="s">
+      <c r="H1" s="5"/>
+      <c r="L1" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="M1" s="2"/>
-      <c r="Q1" s="4" t="s">
+      <c r="M1" s="5"/>
+      <c r="Q1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="R1" s="4"/>
+      <c r="R1" s="3"/>
       <c r="U1" s="1"/>
-      <c r="V1" s="5" t="s">
+      <c r="V1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="W1" s="5" t="s">
+      <c r="W1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="X1" s="5" t="s">
+      <c r="X1" s="4" t="s">
         <v>6</v>
       </c>
     </row>
@@ -14997,7 +15000,7 @@
       <c r="S2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="U2" s="5" t="s">
+      <c r="U2" s="4" t="s">
         <v>7</v>
       </c>
       <c r="V2" s="1">
@@ -15062,7 +15065,7 @@
       <c r="S3" s="1">
         <v>4.1025599999999999E-3</v>
       </c>
-      <c r="U3" s="5" t="s">
+      <c r="U3" s="4" t="s">
         <v>8</v>
       </c>
       <c r="V3" s="1">
@@ -15127,7 +15130,7 @@
       <c r="S4" s="1">
         <v>3.4421389999999999E-3</v>
       </c>
-      <c r="U4" s="5" t="s">
+      <c r="U4" s="4" t="s">
         <v>9</v>
       </c>
       <c r="V4" s="1">
@@ -15192,7 +15195,7 @@
       <c r="S5" s="1">
         <v>3.8480200000000002E-3</v>
       </c>
-      <c r="U5" s="5" t="s">
+      <c r="U5" s="4" t="s">
         <v>10</v>
       </c>
       <c r="V5" s="1">
@@ -15254,8 +15257,23 @@
       <c r="R6" s="1">
         <v>939</v>
       </c>
-      <c r="S6" s="3">
+      <c r="S6" s="2">
         <v>9.7987399999999994E-4</v>
+      </c>
+      <c r="U6" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="V6">
+        <f>MIN(V2:V5)</f>
+        <v>1135.24</v>
+      </c>
+      <c r="W6">
+        <f t="shared" ref="W6:X6" si="0">MIN(W2:W5)</f>
+        <v>4419.46</v>
+      </c>
+      <c r="X6">
+        <f t="shared" si="0"/>
+        <v>18955.36</v>
       </c>
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.3">
@@ -15754,7 +15772,7 @@
       <c r="R16" s="1">
         <v>240</v>
       </c>
-      <c r="S16" s="3">
+      <c r="S16" s="2">
         <v>7.9790199999999996E-4</v>
       </c>
     </row>
@@ -15892,7 +15910,7 @@
       <c r="M19" s="1">
         <v>710</v>
       </c>
-      <c r="N19" s="3">
+      <c r="N19" s="2">
         <v>9.6674599999999999E-4</v>
       </c>
       <c r="P19" s="1">
@@ -15904,7 +15922,7 @@
       <c r="R19" s="1">
         <v>1845</v>
       </c>
-      <c r="S19" s="3">
+      <c r="S19" s="2">
         <v>6.5130400000000001E-4</v>
       </c>
     </row>
@@ -15918,7 +15936,7 @@
       <c r="C20" s="1">
         <v>744</v>
       </c>
-      <c r="D20" s="3">
+      <c r="D20" s="2">
         <v>9.6929799999999995E-4</v>
       </c>
       <c r="F20" s="1">
@@ -15992,7 +16010,7 @@
       <c r="M21" s="1">
         <v>308</v>
       </c>
-      <c r="N21" s="3">
+      <c r="N21" s="2">
         <v>9.8060300000000003E-4</v>
       </c>
       <c r="P21" s="1">
@@ -16054,7 +16072,7 @@
       <c r="R22" s="1">
         <v>938</v>
       </c>
-      <c r="S22" s="3">
+      <c r="S22" s="2">
         <v>7.7747999999999999E-4</v>
       </c>
     </row>
@@ -16130,7 +16148,7 @@
       <c r="H24" s="1">
         <v>883</v>
       </c>
-      <c r="I24" s="3">
+      <c r="I24" s="2">
         <v>9.6273400000000003E-4</v>
       </c>
       <c r="K24" s="1">
@@ -16154,7 +16172,7 @@
       <c r="R24" s="1">
         <v>883</v>
       </c>
-      <c r="S24" s="3">
+      <c r="S24" s="2">
         <v>7.7237599999999997E-4</v>
       </c>
     </row>
@@ -16218,7 +16236,7 @@
       <c r="C26" s="1">
         <v>271</v>
       </c>
-      <c r="D26" s="3">
+      <c r="D26" s="2">
         <v>5.4226700000000003E-4</v>
       </c>
       <c r="F26" s="1">
@@ -16242,7 +16260,7 @@
       <c r="M26" s="1">
         <v>932</v>
       </c>
-      <c r="N26" s="3">
+      <c r="N26" s="2">
         <v>8.6062599999999997E-4</v>
       </c>
       <c r="P26" s="1">
@@ -16254,7 +16272,7 @@
       <c r="R26" s="1">
         <v>1637</v>
       </c>
-      <c r="S26" s="3">
+      <c r="S26" s="2">
         <v>5.8821600000000002E-4</v>
       </c>
     </row>
@@ -16318,7 +16336,7 @@
       <c r="C28" s="1">
         <v>399</v>
       </c>
-      <c r="D28" s="3">
+      <c r="D28" s="2">
         <v>7.0418100000000001E-4</v>
       </c>
       <c r="F28" s="1">
@@ -16330,7 +16348,7 @@
       <c r="H28" s="1">
         <v>898</v>
       </c>
-      <c r="I28" s="3">
+      <c r="I28" s="2">
         <v>9.7075700000000004E-4</v>
       </c>
       <c r="K28" s="1">
@@ -16354,7 +16372,7 @@
       <c r="R28" s="1">
         <v>898</v>
       </c>
-      <c r="S28" s="3">
+      <c r="S28" s="2">
         <v>7.6252899999999996E-4</v>
       </c>
     </row>
@@ -16404,7 +16422,7 @@
       <c r="R29" s="1">
         <v>1292</v>
       </c>
-      <c r="S29" s="3">
+      <c r="S29" s="2">
         <v>9.2334999999999997E-4</v>
       </c>
     </row>
@@ -16554,7 +16572,7 @@
       <c r="R32" s="1">
         <v>916</v>
       </c>
-      <c r="S32" s="3">
+      <c r="S32" s="2">
         <v>8.7448400000000003E-4</v>
       </c>
     </row>
@@ -16580,7 +16598,7 @@
       <c r="H33" s="1">
         <v>803</v>
       </c>
-      <c r="I33" s="3">
+      <c r="I33" s="2">
         <v>8.6791899999999998E-4</v>
       </c>
       <c r="K33" s="1">
@@ -16604,7 +16622,7 @@
       <c r="R33" s="1">
         <v>803</v>
       </c>
-      <c r="S33" s="3">
+      <c r="S33" s="2">
         <v>7.0272300000000004E-4</v>
       </c>
     </row>
@@ -16680,7 +16698,7 @@
       <c r="H35" s="1">
         <v>528</v>
       </c>
-      <c r="I35" s="3">
+      <c r="I35" s="2">
         <v>9.3538400000000004E-4</v>
       </c>
       <c r="K35" s="1">
@@ -16704,7 +16722,7 @@
       <c r="R35" s="1">
         <v>528</v>
       </c>
-      <c r="S35" s="3">
+      <c r="S35" s="2">
         <v>7.1293400000000003E-4</v>
       </c>
     </row>
@@ -16830,7 +16848,7 @@
       <c r="H38" s="1">
         <v>707</v>
       </c>
-      <c r="I38" s="3">
+      <c r="I38" s="2">
         <v>9.7914399999999993E-4</v>
       </c>
       <c r="K38" s="1">
@@ -16854,7 +16872,7 @@
       <c r="R38" s="1">
         <v>707</v>
       </c>
-      <c r="S38" s="3">
+      <c r="S38" s="2">
         <v>9.2298499999999997E-4</v>
       </c>
     </row>
@@ -16918,7 +16936,7 @@
       <c r="C40" s="1">
         <v>565</v>
       </c>
-      <c r="D40" s="3">
+      <c r="D40" s="2">
         <v>7.6872799999999999E-4</v>
       </c>
       <c r="F40" s="1">
@@ -16930,7 +16948,7 @@
       <c r="H40" s="1">
         <v>835</v>
       </c>
-      <c r="I40" s="3">
+      <c r="I40" s="2">
         <v>9.3720700000000001E-4</v>
       </c>
       <c r="K40" s="1">
@@ -16954,7 +16972,7 @@
       <c r="R40" s="1">
         <v>835</v>
       </c>
-      <c r="S40" s="3">
+      <c r="S40" s="2">
         <v>6.6589100000000005E-4</v>
       </c>
     </row>
@@ -17004,7 +17022,7 @@
       <c r="R41" s="1">
         <v>1213</v>
       </c>
-      <c r="S41" s="3">
+      <c r="S41" s="2">
         <v>9.5288800000000004E-4</v>
       </c>
     </row>
@@ -17018,7 +17036,7 @@
       <c r="C42" s="1">
         <v>431</v>
       </c>
-      <c r="D42" s="3">
+      <c r="D42" s="2">
         <v>6.8193699999999997E-4</v>
       </c>
       <c r="F42" s="1">
@@ -17054,7 +17072,7 @@
       <c r="R42" s="1">
         <v>2009</v>
       </c>
-      <c r="S42" s="3">
+      <c r="S42" s="2">
         <v>5.4482E-4</v>
       </c>
     </row>
@@ -17068,7 +17086,7 @@
       <c r="C43" s="1">
         <v>455</v>
       </c>
-      <c r="D43" s="3">
+      <c r="D43" s="2">
         <v>5.0798800000000002E-4</v>
       </c>
       <c r="F43" s="1">
@@ -17080,7 +17098,7 @@
       <c r="H43" s="1">
         <v>505</v>
       </c>
-      <c r="I43" s="3">
+      <c r="I43" s="2">
         <v>5.0142399999999999E-4</v>
       </c>
       <c r="K43" s="1">
@@ -17104,7 +17122,7 @@
       <c r="R43" s="1">
         <v>505</v>
       </c>
-      <c r="S43" s="3">
+      <c r="S43" s="2">
         <v>4.06244E-4</v>
       </c>
     </row>
@@ -17118,7 +17136,7 @@
       <c r="C44" s="1">
         <v>664</v>
       </c>
-      <c r="D44" s="3">
+      <c r="D44" s="2">
         <v>7.0819299999999997E-4</v>
       </c>
       <c r="F44" s="1">
@@ -17130,7 +17148,7 @@
       <c r="H44" s="1">
         <v>874</v>
       </c>
-      <c r="I44" s="3">
+      <c r="I44" s="2">
         <v>7.7128099999999996E-4</v>
       </c>
       <c r="K44" s="1">
@@ -17142,7 +17160,7 @@
       <c r="M44" s="1">
         <v>707</v>
       </c>
-      <c r="N44" s="3">
+      <c r="N44" s="2">
         <v>7.1184000000000004E-4</v>
       </c>
       <c r="P44" s="1">
@@ -17154,7 +17172,7 @@
       <c r="R44" s="1">
         <v>874</v>
       </c>
-      <c r="S44" s="3">
+      <c r="S44" s="2">
         <v>7.3517899999999998E-4</v>
       </c>
     </row>
@@ -17168,7 +17186,7 @@
       <c r="C45" s="1">
         <v>389</v>
       </c>
-      <c r="D45" s="3">
+      <c r="D45" s="2">
         <v>5.6633599999999997E-4</v>
       </c>
       <c r="F45" s="1">
@@ -17180,7 +17198,7 @@
       <c r="H45" s="1">
         <v>958</v>
       </c>
-      <c r="I45" s="3">
+      <c r="I45" s="2">
         <v>7.77116E-4</v>
       </c>
       <c r="K45" s="1">
@@ -17204,7 +17222,7 @@
       <c r="R45" s="1">
         <v>958</v>
       </c>
-      <c r="S45" s="3">
+      <c r="S45" s="2">
         <v>5.5575999999999998E-4</v>
       </c>
     </row>
@@ -17218,7 +17236,7 @@
       <c r="C46" s="1">
         <v>772</v>
       </c>
-      <c r="D46" s="3">
+      <c r="D46" s="2">
         <v>7.4320199999999999E-4</v>
       </c>
       <c r="F46" s="1">
@@ -17230,7 +17248,7 @@
       <c r="H46" s="1">
         <v>841</v>
       </c>
-      <c r="I46" s="3">
+      <c r="I46" s="2">
         <v>7.4283599999999997E-4</v>
       </c>
       <c r="K46" s="1">
@@ -17254,7 +17272,7 @@
       <c r="R46" s="1">
         <v>841</v>
       </c>
-      <c r="S46" s="3">
+      <c r="S46" s="2">
         <v>6.1009599999999997E-4</v>
       </c>
     </row>
@@ -17268,7 +17286,7 @@
       <c r="C47" s="1">
         <v>194</v>
       </c>
-      <c r="D47" s="3">
+      <c r="D47" s="2">
         <v>2.7933899999999998E-4</v>
       </c>
       <c r="F47" s="1">
@@ -17280,7 +17298,7 @@
       <c r="H47" s="1">
         <v>1960</v>
       </c>
-      <c r="I47" s="3">
+      <c r="I47" s="2">
         <v>9.5835799999999997E-4</v>
       </c>
       <c r="K47" s="1">
@@ -17292,7 +17310,7 @@
       <c r="M47" s="1">
         <v>598</v>
       </c>
-      <c r="N47" s="3">
+      <c r="N47" s="2">
         <v>4.4453599999999999E-4</v>
       </c>
       <c r="P47" s="1">
@@ -17304,7 +17322,7 @@
       <c r="R47" s="1">
         <v>1960</v>
       </c>
-      <c r="S47" s="3">
+      <c r="S47" s="2">
         <v>2.6985699999999997E-4</v>
       </c>
     </row>
@@ -17354,7 +17372,7 @@
       <c r="R48" s="1">
         <v>1363</v>
       </c>
-      <c r="S48" s="3">
+      <c r="S48" s="2">
         <v>8.9672799999999996E-4</v>
       </c>
     </row>
@@ -17380,7 +17398,7 @@
       <c r="H49" s="1">
         <v>969</v>
       </c>
-      <c r="I49" s="3">
+      <c r="I49" s="2">
         <v>8.7740099999999998E-4</v>
       </c>
       <c r="K49" s="1">
@@ -17404,7 +17422,7 @@
       <c r="R49" s="1">
         <v>969</v>
       </c>
-      <c r="S49" s="3">
+      <c r="S49" s="2">
         <v>6.7865500000000001E-4</v>
       </c>
     </row>
@@ -17454,7 +17472,7 @@
       <c r="R50" s="1">
         <v>1623</v>
       </c>
-      <c r="S50" s="3">
+      <c r="S50" s="2">
         <v>9.37936E-4</v>
       </c>
     </row>
@@ -17480,7 +17498,7 @@
       <c r="H51" s="1">
         <v>1068</v>
       </c>
-      <c r="I51" s="3">
+      <c r="I51" s="2">
         <v>9.29914E-4</v>
       </c>
       <c r="K51" s="1">
@@ -17504,7 +17522,7 @@
       <c r="R51" s="1">
         <v>1068</v>
       </c>
-      <c r="S51" s="3">
+      <c r="S51" s="2">
         <v>7.24239E-4</v>
       </c>
     </row>
@@ -17518,7 +17536,7 @@
       <c r="C52" s="1">
         <v>756</v>
       </c>
-      <c r="D52" s="3">
+      <c r="D52" s="2">
         <v>5.4700799999999998E-4</v>
       </c>
       <c r="F52" s="1">
@@ -17530,7 +17548,7 @@
       <c r="H52" s="1">
         <v>782</v>
       </c>
-      <c r="I52" s="3">
+      <c r="I52" s="2">
         <v>5.3460900000000002E-4</v>
       </c>
       <c r="K52" s="1">
@@ -17542,7 +17560,7 @@
       <c r="M52" s="1">
         <v>225</v>
       </c>
-      <c r="N52" s="3">
+      <c r="N52" s="2">
         <v>3.1872399999999999E-4</v>
       </c>
       <c r="P52" s="1">
@@ -17554,7 +17572,7 @@
       <c r="R52" s="1">
         <v>782</v>
       </c>
-      <c r="S52" s="3">
+      <c r="S52" s="2">
         <v>3.2382899999999998E-4</v>
       </c>
     </row>
@@ -19780,7 +19798,7 @@
       <c r="H97" s="1">
         <v>627</v>
       </c>
-      <c r="I97" s="3">
+      <c r="I97" s="2">
         <v>6.43646E-4</v>
       </c>
       <c r="K97" s="1">
@@ -19804,7 +19822,7 @@
       <c r="R97" s="1">
         <v>627</v>
       </c>
-      <c r="S97" s="3">
+      <c r="S97" s="2">
         <v>6.43646E-4</v>
       </c>
     </row>
@@ -19904,7 +19922,7 @@
       <c r="R99" s="1">
         <v>6039</v>
       </c>
-      <c r="S99" s="3">
+      <c r="S99" s="2">
         <v>9.5507600000000002E-4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Removed unused method from Robert
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="828" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="830" uniqueCount="14">
   <si>
     <t>MazeNumber</t>
   </si>
@@ -64,6 +64,9 @@
   </si>
   <si>
     <t>Crazy</t>
+  </si>
+  <si>
+    <t>Max</t>
   </si>
 </sst>
 </file>
@@ -107,7 +110,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -124,6 +127,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -41393,10 +41400,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:X202"/>
+  <dimension ref="A1:Y202"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="X6" sqref="X6"/>
+      <selection activeCell="Y8" sqref="Y8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -41423,23 +41430,23 @@
     <col min="21" max="21" width="19.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="B1" s="5" t="s">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="B1" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="5"/>
-      <c r="G1" s="5" t="s">
+      <c r="C1" s="6"/>
+      <c r="G1" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="H1" s="5"/>
-      <c r="L1" s="5" t="s">
+      <c r="H1" s="6"/>
+      <c r="L1" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="M1" s="5"/>
-      <c r="Q1" s="5" t="s">
+      <c r="M1" s="6"/>
+      <c r="Q1" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="R1" s="5"/>
+      <c r="R1" s="6"/>
       <c r="U1" s="1"/>
       <c r="V1" s="3" t="s">
         <v>4</v>
@@ -41450,8 +41457,11 @@
       <c r="X1" s="3" t="s">
         <v>6</v>
       </c>
+      <c r="Y1" s="7" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
@@ -41515,8 +41525,12 @@
         <f>AVERAGE(C103:C152)</f>
         <v>19786.82</v>
       </c>
+      <c r="Y2" s="5">
+        <f>AVERAGE(C153:C202)</f>
+        <v>1152529.3999999999</v>
+      </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A3" s="4">
         <v>1</v>
       </c>
@@ -41580,8 +41594,12 @@
         <f>AVERAGE(H103:H152)</f>
         <v>18955.36</v>
       </c>
+      <c r="Y3" s="5">
+        <f>AVERAGE(H154:H203)</f>
+        <v>1023260.4489795918</v>
+      </c>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A4" s="4">
         <v>2</v>
       </c>
@@ -41645,8 +41663,12 @@
         <f>AVERAGE(M103:M152)</f>
         <v>20732.82</v>
       </c>
+      <c r="Y4" s="5">
+        <f>AVERAGE(M155:M204)</f>
+        <v>1152657.6041666667</v>
+      </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A5" s="4">
         <v>3</v>
       </c>
@@ -41710,8 +41732,12 @@
         <f>AVERAGE(R103:R152)</f>
         <v>7420</v>
       </c>
+      <c r="Y5" s="5">
+        <f>AVERAGE(R156:R205)</f>
+        <v>363357.55319148937</v>
+      </c>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A6" s="4">
         <v>4</v>
       </c>
@@ -41772,11 +41798,15 @@
         <v>2115.84</v>
       </c>
       <c r="X6">
-        <f t="shared" ref="W6:X6" si="0">MIN(X2:X5)</f>
+        <f t="shared" ref="X6:Y7" si="0">MIN(X2:X5)</f>
         <v>7420</v>
       </c>
+      <c r="Y6">
+        <f t="shared" si="0"/>
+        <v>363357.55319148937</v>
+      </c>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A7" s="4">
         <v>5</v>
       </c>
@@ -41825,8 +41855,27 @@
       <c r="S7" s="2">
         <v>6.0280200000000005E-4</v>
       </c>
+      <c r="U7" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="V7">
+        <f>MAX(V3:V6)</f>
+        <v>1157.8800000000001</v>
+      </c>
+      <c r="W7">
+        <f>MAX(W3:W6)</f>
+        <v>4852.46</v>
+      </c>
+      <c r="X7">
+        <f>MAX(X3:X6)</f>
+        <v>20732.82</v>
+      </c>
+      <c r="Y7">
+        <f>MAX(Y3:Y6)</f>
+        <v>1152657.6041666667</v>
+      </c>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A8" s="4">
         <v>6</v>
       </c>
@@ -41876,7 +41925,7 @@
         <v>5.2804499999999999E-4</v>
       </c>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A9" s="4">
         <v>7</v>
       </c>
@@ -41926,7 +41975,7 @@
         <v>9.5908699999999996E-4</v>
       </c>
     </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A10" s="4">
         <v>8</v>
       </c>
@@ -41976,7 +42025,7 @@
         <v>9.3611300000000003E-4</v>
       </c>
     </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A11" s="4">
         <v>9</v>
       </c>
@@ -42026,7 +42075,7 @@
         <v>6.5568099999999997E-4</v>
       </c>
     </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A12" s="4">
         <v>10</v>
       </c>
@@ -42076,7 +42125,7 @@
         <v>7.7820999999999999E-4</v>
       </c>
     </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A13" s="4">
         <v>11</v>
       </c>
@@ -42126,7 +42175,7 @@
         <v>7.1038099999999995E-4</v>
       </c>
     </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A14" s="4">
         <v>12</v>
       </c>
@@ -42176,7 +42225,7 @@
         <v>1.6092979999999999E-3</v>
       </c>
     </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A15" s="4">
         <v>13</v>
       </c>
@@ -42226,7 +42275,7 @@
         <v>7.9206800000000005E-4</v>
       </c>
     </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A16" s="4">
         <v>14</v>
       </c>

</xml_diff>